<commit_message>
fix: fecha autorizacion formato dd-mmm-yy, motivo sin duplicados, excluir incapacidad, pasar quincena params al excel
</commit_message>
<xml_diff>
--- a/webapp/output/mobper/MobPer_8490_20260201.xlsx
+++ b/webapp/output/mobper/MobPer_8490_20260201.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raulc\Downloads\debug biostar para checadores\webapp\output\mobper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5358521E-A336-4E15-88DF-E554C8C5492C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DFCF49-DDFE-4DF6-825A-D8BC58516863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="3360" windowWidth="17280" windowHeight="8880" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="100">
   <si>
     <t>Fecha de Autorizacion</t>
   </si>
@@ -338,6 +338,12 @@
     <t>DISEÑO</t>
   </si>
   <si>
+    <t>5 de febrero</t>
+  </si>
+  <si>
+    <t>5 falta justificada, trabajo remoto.</t>
+  </si>
+  <si>
     <t>Raúl Cetina</t>
   </si>
 </sst>
@@ -350,7 +356,7 @@
     <numFmt numFmtId="164" formatCode="[$$-80A]#,##0.00;[Red]\-[$$-80A]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$$-80A]#,##0.00;\-[$$-80A]#,##0.00"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -501,6 +507,13 @@
       <b/>
       <i/>
       <sz val="8"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
@@ -856,7 +869,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="231">
+  <cellXfs count="232">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1429,6 +1442,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3029,7 +3045,9 @@
         <a:prstGeom prst="ellipse">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
+        <a:solidFill>
+          <a:srgbClr val="000000"/>
+        </a:solidFill>
         <a:ln w="9525">
           <a:solidFill>
             <a:srgbClr val="000000"/>
@@ -3038,15 +3056,6 @@
           <a:headEnd/>
           <a:tailEnd/>
         </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
       <xdr:txBody>
         <a:bodyPr/>
@@ -8966,7 +8975,7 @@
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="198">
-        <v>46175</v>
+        <v>46059</v>
       </c>
       <c r="I10" s="158"/>
       <c r="J10" s="158"/>
@@ -8977,7 +8986,9 @@
       </c>
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
-      <c r="P10" s="156"/>
+      <c r="P10" s="231" t="s">
+        <v>97</v>
+      </c>
       <c r="Q10" s="199"/>
       <c r="R10" s="199"/>
       <c r="S10" s="39"/>
@@ -9112,7 +9123,9 @@
       <c r="D20" s="90"/>
       <c r="E20" s="90"/>
       <c r="F20" s="10"/>
-      <c r="G20" s="138"/>
+      <c r="G20" s="138" t="s">
+        <v>98</v>
+      </c>
       <c r="H20" s="139"/>
       <c r="I20" s="139"/>
       <c r="J20" s="139"/>
@@ -10020,7 +10033,7 @@
       </c>
       <c r="D56" s="8"/>
       <c r="E56" s="104" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F56" s="104"/>
       <c r="G56" s="104"/>

</xml_diff>